<commit_message>
Add OCM example codes.
</commit_message>
<xml_diff>
--- a/MR Thermometry/PRF Based/DataBase.xlsx
+++ b/MR Thermometry/PRF Based/DataBase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49A9B1A-26A0-4FB4-B53B-FEF06CA32D1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98425D0A-AD74-40FC-A80E-3B97C21125F1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,388 +191,388 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="128"/>
                 <c:pt idx="0">
-                  <c:v>1.0115134284453813</c:v>
+                  <c:v>1.2839619078076006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0119047437993929</c:v>
+                  <c:v>1.2820313768228686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0109884628178532</c:v>
+                  <c:v>1.2826649661370233</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.010536210553866</c:v>
+                  <c:v>1.2842420606547471</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0109232349618555</c:v>
+                  <c:v>1.2847638822679366</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.011093532968723</c:v>
+                  <c:v>1.2850974165553222</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0111115098913921</c:v>
+                  <c:v>1.2852476066968794</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0111034636205389</c:v>
+                  <c:v>1.2854841668937307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.011107084958258</c:v>
+                  <c:v>1.285781180520565</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0110908641177736</c:v>
+                  <c:v>1.2860837678522883</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0109830921044949</c:v>
+                  <c:v>1.286279439263043</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0107814979934493</c:v>
+                  <c:v>1.2864429717345287</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0105109477204128</c:v>
+                  <c:v>1.2867249088420087</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0102352961090635</c:v>
+                  <c:v>1.2870499574310865</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0099973615893509</c:v>
+                  <c:v>1.2873123125030308</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0098191390562785</c:v>
+                  <c:v>1.2876201625059984</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0097059315460721</c:v>
+                  <c:v>1.2880220225156231</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0096169231074672</c:v>
+                  <c:v>1.2883267313917</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0095525912905592</c:v>
+                  <c:v>1.2884578632178898</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0095432430753934</c:v>
+                  <c:v>1.2886069897471431</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0096279031516067</c:v>
+                  <c:v>1.2887621285491022</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0097776376823349</c:v>
+                  <c:v>1.2887131012138262</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0099452510051854</c:v>
+                  <c:v>1.2885416325833878</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.0101405887692054</c:v>
+                  <c:v>1.2884153780511634</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0103508285845264</c:v>
+                  <c:v>1.2881536934952147</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.0105691621462705</c:v>
+                  <c:v>1.2876405424693611</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.0107763063517203</c:v>
+                  <c:v>1.2871213531680235</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.0110349949804844</c:v>
+                  <c:v>1.2866995418817593</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.01137198641134</c:v>
+                  <c:v>1.2861829200464261</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0117961265945166</c:v>
+                  <c:v>1.2856496939011499</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0122861089436272</c:v>
+                  <c:v>1.2853913388539069</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.0128636096806136</c:v>
+                  <c:v>1.2852826135476347</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.013539920541292</c:v>
+                  <c:v>1.2850987066950266</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.0142699098320849</c:v>
+                  <c:v>1.2850411919326783</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0149991043195032</c:v>
+                  <c:v>1.2853026582794551</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.0156764929960027</c:v>
+                  <c:v>1.2855560259572663</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0162984840924085</c:v>
+                  <c:v>1.2856978183993546</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.0168438258612478</c:v>
+                  <c:v>1.2860622541208446</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.0172996565226387</c:v>
+                  <c:v>1.2865393352881642</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.0177352545736087</c:v>
+                  <c:v>1.2867277844354743</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.018106399643494</c:v>
+                  <c:v>1.2868305300116485</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.0184081791336648</c:v>
+                  <c:v>1.2871882391203229</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.0186017218383605</c:v>
+                  <c:v>1.2874857690650416</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.0188165152621811</c:v>
+                  <c:v>1.2874780087742774</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0190128712259099</c:v>
+                  <c:v>1.2877074784915357</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.0191577411599844</c:v>
+                  <c:v>1.288263178387733</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.0191939887477952</c:v>
+                  <c:v>1.2884844136257925</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.0192214512409332</c:v>
+                  <c:v>1.2885259991809925</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.0191720904686574</c:v>
+                  <c:v>1.2890317768670045</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.0187530875024648</c:v>
+                  <c:v>1.28970382458118</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.0181846024065069</c:v>
+                  <c:v>1.2895852033705637</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.0174464732656487</c:v>
+                  <c:v>1.2896239983763433</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.0169652642303719</c:v>
+                  <c:v>1.2907835010906612</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.0158386955509484</c:v>
+                  <c:v>1.2911956712614487</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.0143643029089588</c:v>
+                  <c:v>1.2898988396442035</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.0138980377522586</c:v>
+                  <c:v>1.289378140390123</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.0149645122214674</c:v>
+                  <c:v>1.2930092905827739</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.0174460455856695</c:v>
+                  <c:v>1.2973808620854579</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.0129271418984716</c:v>
+                  <c:v>1.2891697066395778</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.98941661702920269</c:v>
+                  <c:v>1.25517031344254</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.94282172634129424</c:v>
+                  <c:v>1.1916102682465772</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.8753852382269659</c:v>
+                  <c:v>1.1013556654239387</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.79008836156844953</c:v>
+                  <c:v>0.98843717823108435</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.69027550540457627</c:v>
+                  <c:v>0.85791110904563528</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.58110649127087421</c:v>
+                  <c:v>0.716128256138026</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.46825470703787436</c:v>
+                  <c:v>0.57100841681762105</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.35767212759562372</c:v>
+                  <c:v>0.43026535379965947</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.25370275515488627</c:v>
+                  <c:v>0.29958293472314435</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.16177013490859751</c:v>
+                  <c:v>0.18475335042820601</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>8.7967025240660884E-2</c:v>
+                  <c:v>9.3144325004473311E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.6590479061141136E-2</c:v>
+                  <c:v>3.3213200886100816E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.2541290385684207E-2</c:v>
+                  <c:v>1.0967165963481443E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.1359972532098998E-2</c:v>
+                  <c:v>1.3722424800549336E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.1913040665704451E-2</c:v>
+                  <c:v>1.6318462518791477E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.230189986355381E-2</c:v>
+                  <c:v>1.7974431423696102E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.2862070211557591E-2</c:v>
+                  <c:v>1.8429179625326798E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.332985001113487E-2</c:v>
+                  <c:v>1.7915661419244184E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.3794656784102029E-2</c:v>
+                  <c:v>1.7546006399103302E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.4128699714233521E-2</c:v>
+                  <c:v>1.7611050297955504E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.4232079165133771E-2</c:v>
+                  <c:v>1.7379577309042611E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.4332834980516133E-2</c:v>
+                  <c:v>1.6794383773883478E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.4537081625494828E-2</c:v>
+                  <c:v>1.6464758079946185E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.4762755717502065E-2</c:v>
+                  <c:v>1.6254935011613993E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.5007472363082287E-2</c:v>
+                  <c:v>1.5648544148270313E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.5326377164137702E-2</c:v>
+                  <c:v>1.4998340940173573E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.5700002388396462E-2</c:v>
+                  <c:v>1.4713142424327577E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.599733919233812E-2</c:v>
+                  <c:v>1.4396328831566201E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.6147931999402627E-2</c:v>
+                  <c:v>1.3832375688065873E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.6181313228736029E-2</c:v>
+                  <c:v>1.3419516928953563E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.6078375179689273E-2</c:v>
+                  <c:v>1.3234165612613811E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.5772348547485097E-2</c:v>
+                  <c:v>1.2886857239050089E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.5267672682660169E-2</c:v>
+                  <c:v>1.2483309790142097E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.4605500991221314E-2</c:v>
+                  <c:v>1.2415871599016682E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.3826999730022507E-2</c:v>
+                  <c:v>1.2509818761734645E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.3009957845412371E-2</c:v>
+                  <c:v>1.2453405291067813E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.2197048409775283E-2</c:v>
+                  <c:v>1.2406306602465833E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.1432801877867924E-2</c:v>
+                  <c:v>1.2490288676885024E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.0720893115836379E-2</c:v>
+                  <c:v>1.240432310537095E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.0021903537525745E-2</c:v>
+                  <c:v>1.2092249748865923E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>9.3702919016233916E-3</c:v>
+                  <c:v>1.1865845488122372E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>8.8105416776056052E-3</c:v>
+                  <c:v>1.1702652298894077E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>8.3502236466336029E-3</c:v>
+                  <c:v>1.1350724871890532E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>7.959270322797217E-3</c:v>
+                  <c:v>1.0914819267582027E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>7.5845807326742447E-3</c:v>
+                  <c:v>1.0581444670971121E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>7.2321591610891639E-3</c:v>
+                  <c:v>1.0170204026836235E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>6.9188936408589377E-3</c:v>
+                  <c:v>9.570446092995134E-3</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>6.619186862732513E-3</c:v>
+                  <c:v>9.0635157076655263E-3</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>6.3285729108833828E-3</c:v>
+                  <c:v>8.7208421428913094E-3</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>6.0595820791816205E-3</c:v>
+                  <c:v>8.2588316848120399E-3</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>5.7835213247718854E-3</c:v>
+                  <c:v>7.6250879935456997E-3</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>5.4613156013766633E-3</c:v>
+                  <c:v>6.9972957908531284E-3</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>5.1007602821217879E-3</c:v>
+                  <c:v>6.3436453995575149E-3</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>4.7172570377172745E-3</c:v>
+                  <c:v>5.576819267765847E-3</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>4.2889111962293907E-3</c:v>
+                  <c:v>4.8633595400045838E-3</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3.8427480695276783E-3</c:v>
+                  <c:v>4.3993299681788466E-3</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>3.4407523073605928E-3</c:v>
+                  <c:v>4.1500818731578766E-3</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>3.108794292932344E-3</c:v>
+                  <c:v>3.9460160489655114E-3</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.8487383011450828E-3</c:v>
+                  <c:v>3.7727127334954724E-3</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2.6502782511110897E-3</c:v>
+                  <c:v>3.6878979914241219E-3</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2.472259630182373E-3</c:v>
+                  <c:v>3.5398602637655412E-3</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2.3153581737762881E-3</c:v>
+                  <c:v>3.1697854404337624E-3</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.2722118247088707E-3</c:v>
+                  <c:v>2.8551751872644931E-3</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2.4250084856544474E-3</c:v>
+                  <c:v>2.0919967401155709E-3</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2.7384463208427246E-3</c:v>
+                  <c:v>1.4506102076251534E-3</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.6238710193214037E-3</c:v>
+                  <c:v>1.3832961078920456E-3</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.0868220170835402E-3</c:v>
+                  <c:v>2.2588015623985205E-3</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1.5506197938589374E-3</c:v>
+                  <c:v>4.252371007999689E-3</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>5.8284113752022978E-36</c:v>
+                  <c:v>1.5758492296649355E-35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,6 +829,763 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1050">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>k-space</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1050" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Energy Spectrum</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1050">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10066437007874016"/>
+          <c:y val="0.13872688092976704"/>
+          <c:w val="0.85836340769903763"/>
+          <c:h val="0.7550551616732557"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$DX$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="128"/>
+                <c:pt idx="0">
+                  <c:v>1.519658488451147</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5197662801670355</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5226195622660994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5235812900347121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5240720134126584</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5248910393078781</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5251260817414014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5254253961114108</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5257661796513875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5259215584863586</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.526023773655945</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.526172017547349</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5262884334559705</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5262810828200006</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5262067140464013</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5262260218138075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5263592903200114</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5264332998420962</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5263482625615363</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5262315168212166</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.526218619880567</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5262298419365499</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5261144066930949</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.525914017606214</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5257936308946307</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5257680877731492</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.5256736285874044</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5254366384992504</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.525238157644355</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5252266283461062</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.5252862727102734</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5252677354814179</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5252028867443601</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.525263783119333</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5254891446069134</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.5256741010021444</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.525725584647214</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.5257997427397538</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5259888597637279</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5261844070685668</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5262281406358076</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.5261693261253466</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.5262212718246344</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5263529392611872</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.5263822999718129</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5263071966125326</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.5262469615990861</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.5263009545716171</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.5263441887643479</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.5261672201149856</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.5258450132215851</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.5255512281580013</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.5252667502560493</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.5248489251275763</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.5242679496181109</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.5237471962881441</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.5233733099193394</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.5229033942122907</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.5222785850417042</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.5216792138532518</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.5212542403460343</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.5209549915627114</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5205199592891647</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5200168397370246</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.519707154430022</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.5194574975022834</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.5190874952136926</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.5185507372782112</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.5180363211971104</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.5178226360950546</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.5175177493677661</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.5168407007256781</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.516264922054992</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.5159592161431157</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.5157731783138455</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.5154869807734723</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.514851147471598</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.5145529519975212</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.5149961207972011</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.514899886346164</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.5138483742718316</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.513330972420017</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.5141168415135202</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.5149276650750432</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.5136461548980926</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.5101237328779418</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.5077650022151419</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.5107773869134853</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.5183404969291765</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.5207019456865558</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.5031797692426034</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.4557364782864732</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.3763480720795631</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.2670445247921924</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.1321672192063503</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.97877575372190795</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.81508483367078532</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.6487664089452142</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.48668327611806517</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.33602907362330697</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.2062990964860692</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.1083948759173174</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>4.7858324503776598E-2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.8821412515957783E-2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>8.2962639729193578E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>6.8705951520887593E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>8.8793403018316546E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.0059587743578189E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>9.5889398454073373E-3</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>8.4880041080658639E-3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>8.0113458891341218E-3</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>8.3184224271842366E-3</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>8.4818298306327412E-3</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>8.0443360770167723E-3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>7.5316688990723834E-3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>7.6674303139162387E-3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>8.1287947944547884E-3</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>8.1127091917667562E-3</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>7.6323227262003008E-3</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>7.4448976376214164E-3</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>7.7713864060567463E-3</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>7.6875965574549855E-3</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>7.5428638439906459E-3</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>8.7825675002132422E-3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>8.265019327992406E-3</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.2654127611547791E-2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.6125067127777105E-2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>5.5041904752392974E-35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A4F-4D7A-A7E3-C588C85B1496}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="623955456"/>
+        <c:axId val="623955784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="623955456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Nx</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46522801837270339"/>
+              <c:y val="0.92146613968973745"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="623955784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="623955784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Signal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> Intensity</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.1782589676290488E-3"/>
+              <c:y val="0.30944779762451874"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="623955456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -869,7 +1626,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1418,6 +2731,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E3ED5F1-5618-4E9E-8FCD-9A8D7891959B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1689,398 +3038,784 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DX1"/>
+  <dimension ref="A1:DX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1.0115134284453813</v>
+        <v>1.2839619078076006</v>
       </c>
       <c r="B1">
-        <v>1.0119047437993929</v>
+        <v>1.2820313768228686</v>
       </c>
       <c r="C1">
-        <v>1.0109884628178532</v>
+        <v>1.2826649661370233</v>
       </c>
       <c r="D1">
-        <v>1.010536210553866</v>
+        <v>1.2842420606547471</v>
       </c>
       <c r="E1">
-        <v>1.0109232349618555</v>
+        <v>1.2847638822679366</v>
       </c>
       <c r="F1">
-        <v>1.011093532968723</v>
+        <v>1.2850974165553222</v>
       </c>
       <c r="G1">
-        <v>1.0111115098913921</v>
+        <v>1.2852476066968794</v>
       </c>
       <c r="H1">
-        <v>1.0111034636205389</v>
+        <v>1.2854841668937307</v>
       </c>
       <c r="I1">
-        <v>1.011107084958258</v>
+        <v>1.285781180520565</v>
       </c>
       <c r="J1">
-        <v>1.0110908641177736</v>
+        <v>1.2860837678522883</v>
       </c>
       <c r="K1">
-        <v>1.0109830921044949</v>
+        <v>1.286279439263043</v>
       </c>
       <c r="L1">
-        <v>1.0107814979934493</v>
+        <v>1.2864429717345287</v>
       </c>
       <c r="M1">
-        <v>1.0105109477204128</v>
+        <v>1.2867249088420087</v>
       </c>
       <c r="N1">
-        <v>1.0102352961090635</v>
+        <v>1.2870499574310865</v>
       </c>
       <c r="O1">
-        <v>1.0099973615893509</v>
+        <v>1.2873123125030308</v>
       </c>
       <c r="P1">
-        <v>1.0098191390562785</v>
+        <v>1.2876201625059984</v>
       </c>
       <c r="Q1">
-        <v>1.0097059315460721</v>
+        <v>1.2880220225156231</v>
       </c>
       <c r="R1">
-        <v>1.0096169231074672</v>
+        <v>1.2883267313917</v>
       </c>
       <c r="S1">
-        <v>1.0095525912905592</v>
+        <v>1.2884578632178898</v>
       </c>
       <c r="T1">
-        <v>1.0095432430753934</v>
+        <v>1.2886069897471431</v>
       </c>
       <c r="U1">
-        <v>1.0096279031516067</v>
+        <v>1.2887621285491022</v>
       </c>
       <c r="V1">
-        <v>1.0097776376823349</v>
+        <v>1.2887131012138262</v>
       </c>
       <c r="W1">
-        <v>1.0099452510051854</v>
+        <v>1.2885416325833878</v>
       </c>
       <c r="X1">
-        <v>1.0101405887692054</v>
+        <v>1.2884153780511634</v>
       </c>
       <c r="Y1">
-        <v>1.0103508285845264</v>
+        <v>1.2881536934952147</v>
       </c>
       <c r="Z1">
-        <v>1.0105691621462705</v>
+        <v>1.2876405424693611</v>
       </c>
       <c r="AA1">
-        <v>1.0107763063517203</v>
+        <v>1.2871213531680235</v>
       </c>
       <c r="AB1">
-        <v>1.0110349949804844</v>
+        <v>1.2866995418817593</v>
       </c>
       <c r="AC1">
-        <v>1.01137198641134</v>
+        <v>1.2861829200464261</v>
       </c>
       <c r="AD1">
-        <v>1.0117961265945166</v>
+        <v>1.2856496939011499</v>
       </c>
       <c r="AE1">
-        <v>1.0122861089436272</v>
+        <v>1.2853913388539069</v>
       </c>
       <c r="AF1">
-        <v>1.0128636096806136</v>
+        <v>1.2852826135476347</v>
       </c>
       <c r="AG1">
-        <v>1.013539920541292</v>
+        <v>1.2850987066950266</v>
       </c>
       <c r="AH1">
-        <v>1.0142699098320849</v>
+        <v>1.2850411919326783</v>
       </c>
       <c r="AI1">
-        <v>1.0149991043195032</v>
+        <v>1.2853026582794551</v>
       </c>
       <c r="AJ1">
-        <v>1.0156764929960027</v>
+        <v>1.2855560259572663</v>
       </c>
       <c r="AK1">
-        <v>1.0162984840924085</v>
+        <v>1.2856978183993546</v>
       </c>
       <c r="AL1">
-        <v>1.0168438258612478</v>
+        <v>1.2860622541208446</v>
       </c>
       <c r="AM1">
-        <v>1.0172996565226387</v>
+        <v>1.2865393352881642</v>
       </c>
       <c r="AN1">
-        <v>1.0177352545736087</v>
+        <v>1.2867277844354743</v>
       </c>
       <c r="AO1">
-        <v>1.018106399643494</v>
+        <v>1.2868305300116485</v>
       </c>
       <c r="AP1">
-        <v>1.0184081791336648</v>
+        <v>1.2871882391203229</v>
       </c>
       <c r="AQ1">
-        <v>1.0186017218383605</v>
+        <v>1.2874857690650416</v>
       </c>
       <c r="AR1">
-        <v>1.0188165152621811</v>
+        <v>1.2874780087742774</v>
       </c>
       <c r="AS1">
-        <v>1.0190128712259099</v>
+        <v>1.2877074784915357</v>
       </c>
       <c r="AT1">
-        <v>1.0191577411599844</v>
+        <v>1.288263178387733</v>
       </c>
       <c r="AU1">
-        <v>1.0191939887477952</v>
+        <v>1.2884844136257925</v>
       </c>
       <c r="AV1">
-        <v>1.0192214512409332</v>
+        <v>1.2885259991809925</v>
       </c>
       <c r="AW1">
-        <v>1.0191720904686574</v>
+        <v>1.2890317768670045</v>
       </c>
       <c r="AX1">
-        <v>1.0187530875024648</v>
+        <v>1.28970382458118</v>
       </c>
       <c r="AY1">
-        <v>1.0181846024065069</v>
+        <v>1.2895852033705637</v>
       </c>
       <c r="AZ1">
-        <v>1.0174464732656487</v>
+        <v>1.2896239983763433</v>
       </c>
       <c r="BA1">
-        <v>1.0169652642303719</v>
+        <v>1.2907835010906612</v>
       </c>
       <c r="BB1">
-        <v>1.0158386955509484</v>
+        <v>1.2911956712614487</v>
       </c>
       <c r="BC1">
-        <v>1.0143643029089588</v>
+        <v>1.2898988396442035</v>
       </c>
       <c r="BD1">
-        <v>1.0138980377522586</v>
+        <v>1.289378140390123</v>
       </c>
       <c r="BE1">
-        <v>1.0149645122214674</v>
+        <v>1.2930092905827739</v>
       </c>
       <c r="BF1">
-        <v>1.0174460455856695</v>
+        <v>1.2973808620854579</v>
       </c>
       <c r="BG1">
-        <v>1.0129271418984716</v>
+        <v>1.2891697066395778</v>
       </c>
       <c r="BH1">
-        <v>0.98941661702920269</v>
+        <v>1.25517031344254</v>
       </c>
       <c r="BI1">
-        <v>0.94282172634129424</v>
+        <v>1.1916102682465772</v>
       </c>
       <c r="BJ1">
-        <v>0.8753852382269659</v>
+        <v>1.1013556654239387</v>
       </c>
       <c r="BK1">
-        <v>0.79008836156844953</v>
+        <v>0.98843717823108435</v>
       </c>
       <c r="BL1">
-        <v>0.69027550540457627</v>
+        <v>0.85791110904563528</v>
       </c>
       <c r="BM1">
-        <v>0.58110649127087421</v>
+        <v>0.716128256138026</v>
       </c>
       <c r="BN1">
-        <v>0.46825470703787436</v>
+        <v>0.57100841681762105</v>
       </c>
       <c r="BO1">
-        <v>0.35767212759562372</v>
+        <v>0.43026535379965947</v>
       </c>
       <c r="BP1">
-        <v>0.25370275515488627</v>
+        <v>0.29958293472314435</v>
       </c>
       <c r="BQ1">
-        <v>0.16177013490859751</v>
+        <v>0.18475335042820601</v>
       </c>
       <c r="BR1">
-        <v>8.7967025240660884E-2</v>
+        <v>9.3144325004473311E-2</v>
       </c>
       <c r="BS1">
-        <v>3.6590479061141136E-2</v>
+        <v>3.3213200886100816E-2</v>
       </c>
       <c r="BT1">
-        <v>1.2541290385684207E-2</v>
+        <v>1.0967165963481443E-2</v>
       </c>
       <c r="BU1">
-        <v>1.1359972532098998E-2</v>
+        <v>1.3722424800549336E-2</v>
       </c>
       <c r="BV1">
-        <v>1.1913040665704451E-2</v>
+        <v>1.6318462518791477E-2</v>
       </c>
       <c r="BW1">
-        <v>1.230189986355381E-2</v>
+        <v>1.7974431423696102E-2</v>
       </c>
       <c r="BX1">
-        <v>1.2862070211557591E-2</v>
+        <v>1.8429179625326798E-2</v>
       </c>
       <c r="BY1">
-        <v>1.332985001113487E-2</v>
+        <v>1.7915661419244184E-2</v>
       </c>
       <c r="BZ1">
-        <v>1.3794656784102029E-2</v>
+        <v>1.7546006399103302E-2</v>
       </c>
       <c r="CA1">
-        <v>1.4128699714233521E-2</v>
+        <v>1.7611050297955504E-2</v>
       </c>
       <c r="CB1">
-        <v>1.4232079165133771E-2</v>
+        <v>1.7379577309042611E-2</v>
       </c>
       <c r="CC1">
-        <v>1.4332834980516133E-2</v>
+        <v>1.6794383773883478E-2</v>
       </c>
       <c r="CD1">
-        <v>1.4537081625494828E-2</v>
+        <v>1.6464758079946185E-2</v>
       </c>
       <c r="CE1">
-        <v>1.4762755717502065E-2</v>
+        <v>1.6254935011613993E-2</v>
       </c>
       <c r="CF1">
-        <v>1.5007472363082287E-2</v>
+        <v>1.5648544148270313E-2</v>
       </c>
       <c r="CG1">
-        <v>1.5326377164137702E-2</v>
+        <v>1.4998340940173573E-2</v>
       </c>
       <c r="CH1">
-        <v>1.5700002388396462E-2</v>
+        <v>1.4713142424327577E-2</v>
       </c>
       <c r="CI1">
-        <v>1.599733919233812E-2</v>
+        <v>1.4396328831566201E-2</v>
       </c>
       <c r="CJ1">
-        <v>1.6147931999402627E-2</v>
+        <v>1.3832375688065873E-2</v>
       </c>
       <c r="CK1">
-        <v>1.6181313228736029E-2</v>
+        <v>1.3419516928953563E-2</v>
       </c>
       <c r="CL1">
-        <v>1.6078375179689273E-2</v>
+        <v>1.3234165612613811E-2</v>
       </c>
       <c r="CM1">
-        <v>1.5772348547485097E-2</v>
+        <v>1.2886857239050089E-2</v>
       </c>
       <c r="CN1">
-        <v>1.5267672682660169E-2</v>
+        <v>1.2483309790142097E-2</v>
       </c>
       <c r="CO1">
-        <v>1.4605500991221314E-2</v>
+        <v>1.2415871599016682E-2</v>
       </c>
       <c r="CP1">
-        <v>1.3826999730022507E-2</v>
+        <v>1.2509818761734645E-2</v>
       </c>
       <c r="CQ1">
-        <v>1.3009957845412371E-2</v>
+        <v>1.2453405291067813E-2</v>
       </c>
       <c r="CR1">
-        <v>1.2197048409775283E-2</v>
+        <v>1.2406306602465833E-2</v>
       </c>
       <c r="CS1">
-        <v>1.1432801877867924E-2</v>
+        <v>1.2490288676885024E-2</v>
       </c>
       <c r="CT1">
-        <v>1.0720893115836379E-2</v>
+        <v>1.240432310537095E-2</v>
       </c>
       <c r="CU1">
-        <v>1.0021903537525745E-2</v>
+        <v>1.2092249748865923E-2</v>
       </c>
       <c r="CV1">
-        <v>9.3702919016233916E-3</v>
+        <v>1.1865845488122372E-2</v>
       </c>
       <c r="CW1">
-        <v>8.8105416776056052E-3</v>
+        <v>1.1702652298894077E-2</v>
       </c>
       <c r="CX1">
-        <v>8.3502236466336029E-3</v>
+        <v>1.1350724871890532E-2</v>
       </c>
       <c r="CY1">
-        <v>7.959270322797217E-3</v>
+        <v>1.0914819267582027E-2</v>
       </c>
       <c r="CZ1">
-        <v>7.5845807326742447E-3</v>
+        <v>1.0581444670971121E-2</v>
       </c>
       <c r="DA1">
-        <v>7.2321591610891639E-3</v>
+        <v>1.0170204026836235E-2</v>
       </c>
       <c r="DB1">
-        <v>6.9188936408589377E-3</v>
+        <v>9.570446092995134E-3</v>
       </c>
       <c r="DC1">
-        <v>6.619186862732513E-3</v>
+        <v>9.0635157076655263E-3</v>
       </c>
       <c r="DD1">
-        <v>6.3285729108833828E-3</v>
+        <v>8.7208421428913094E-3</v>
       </c>
       <c r="DE1">
-        <v>6.0595820791816205E-3</v>
+        <v>8.2588316848120399E-3</v>
       </c>
       <c r="DF1">
-        <v>5.7835213247718854E-3</v>
+        <v>7.6250879935456997E-3</v>
       </c>
       <c r="DG1">
-        <v>5.4613156013766633E-3</v>
+        <v>6.9972957908531284E-3</v>
       </c>
       <c r="DH1">
-        <v>5.1007602821217879E-3</v>
+        <v>6.3436453995575149E-3</v>
       </c>
       <c r="DI1">
-        <v>4.7172570377172745E-3</v>
+        <v>5.576819267765847E-3</v>
       </c>
       <c r="DJ1">
-        <v>4.2889111962293907E-3</v>
+        <v>4.8633595400045838E-3</v>
       </c>
       <c r="DK1">
-        <v>3.8427480695276783E-3</v>
+        <v>4.3993299681788466E-3</v>
       </c>
       <c r="DL1">
-        <v>3.4407523073605928E-3</v>
+        <v>4.1500818731578766E-3</v>
       </c>
       <c r="DM1">
-        <v>3.108794292932344E-3</v>
+        <v>3.9460160489655114E-3</v>
       </c>
       <c r="DN1">
-        <v>2.8487383011450828E-3</v>
+        <v>3.7727127334954724E-3</v>
       </c>
       <c r="DO1">
-        <v>2.6502782511110897E-3</v>
+        <v>3.6878979914241219E-3</v>
       </c>
       <c r="DP1">
-        <v>2.472259630182373E-3</v>
+        <v>3.5398602637655412E-3</v>
       </c>
       <c r="DQ1">
-        <v>2.3153581737762881E-3</v>
+        <v>3.1697854404337624E-3</v>
       </c>
       <c r="DR1">
-        <v>2.2722118247088707E-3</v>
+        <v>2.8551751872644931E-3</v>
       </c>
       <c r="DS1">
-        <v>2.4250084856544474E-3</v>
+        <v>2.0919967401155709E-3</v>
       </c>
       <c r="DT1">
-        <v>2.7384463208427246E-3</v>
+        <v>1.4506102076251534E-3</v>
       </c>
       <c r="DU1">
-        <v>2.6238710193214037E-3</v>
+        <v>1.3832961078920456E-3</v>
       </c>
       <c r="DV1">
-        <v>2.0868220170835402E-3</v>
+        <v>2.2588015623985205E-3</v>
       </c>
       <c r="DW1">
-        <v>1.5506197938589374E-3</v>
+        <v>4.252371007999689E-3</v>
       </c>
       <c r="DX1">
-        <v>5.8284113752022978E-36</v>
+        <v>1.5758492296649355E-35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:128" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.519658488451147</v>
+      </c>
+      <c r="B2">
+        <v>1.5197662801670355</v>
+      </c>
+      <c r="C2">
+        <v>1.5226195622660994</v>
+      </c>
+      <c r="D2">
+        <v>1.5235812900347121</v>
+      </c>
+      <c r="E2">
+        <v>1.5240720134126584</v>
+      </c>
+      <c r="F2">
+        <v>1.5248910393078781</v>
+      </c>
+      <c r="G2">
+        <v>1.5251260817414014</v>
+      </c>
+      <c r="H2">
+        <v>1.5254253961114108</v>
+      </c>
+      <c r="I2">
+        <v>1.5257661796513875</v>
+      </c>
+      <c r="J2">
+        <v>1.5259215584863586</v>
+      </c>
+      <c r="K2">
+        <v>1.526023773655945</v>
+      </c>
+      <c r="L2">
+        <v>1.526172017547349</v>
+      </c>
+      <c r="M2">
+        <v>1.5262884334559705</v>
+      </c>
+      <c r="N2">
+        <v>1.5262810828200006</v>
+      </c>
+      <c r="O2">
+        <v>1.5262067140464013</v>
+      </c>
+      <c r="P2">
+        <v>1.5262260218138075</v>
+      </c>
+      <c r="Q2">
+        <v>1.5263592903200114</v>
+      </c>
+      <c r="R2">
+        <v>1.5264332998420962</v>
+      </c>
+      <c r="S2">
+        <v>1.5263482625615363</v>
+      </c>
+      <c r="T2">
+        <v>1.5262315168212166</v>
+      </c>
+      <c r="U2">
+        <v>1.526218619880567</v>
+      </c>
+      <c r="V2">
+        <v>1.5262298419365499</v>
+      </c>
+      <c r="W2">
+        <v>1.5261144066930949</v>
+      </c>
+      <c r="X2">
+        <v>1.525914017606214</v>
+      </c>
+      <c r="Y2">
+        <v>1.5257936308946307</v>
+      </c>
+      <c r="Z2">
+        <v>1.5257680877731492</v>
+      </c>
+      <c r="AA2">
+        <v>1.5256736285874044</v>
+      </c>
+      <c r="AB2">
+        <v>1.5254366384992504</v>
+      </c>
+      <c r="AC2">
+        <v>1.525238157644355</v>
+      </c>
+      <c r="AD2">
+        <v>1.5252266283461062</v>
+      </c>
+      <c r="AE2">
+        <v>1.5252862727102734</v>
+      </c>
+      <c r="AF2">
+        <v>1.5252677354814179</v>
+      </c>
+      <c r="AG2">
+        <v>1.5252028867443601</v>
+      </c>
+      <c r="AH2">
+        <v>1.525263783119333</v>
+      </c>
+      <c r="AI2">
+        <v>1.5254891446069134</v>
+      </c>
+      <c r="AJ2">
+        <v>1.5256741010021444</v>
+      </c>
+      <c r="AK2">
+        <v>1.525725584647214</v>
+      </c>
+      <c r="AL2">
+        <v>1.5257997427397538</v>
+      </c>
+      <c r="AM2">
+        <v>1.5259888597637279</v>
+      </c>
+      <c r="AN2">
+        <v>1.5261844070685668</v>
+      </c>
+      <c r="AO2">
+        <v>1.5262281406358076</v>
+      </c>
+      <c r="AP2">
+        <v>1.5261693261253466</v>
+      </c>
+      <c r="AQ2">
+        <v>1.5262212718246344</v>
+      </c>
+      <c r="AR2">
+        <v>1.5263529392611872</v>
+      </c>
+      <c r="AS2">
+        <v>1.5263822999718129</v>
+      </c>
+      <c r="AT2">
+        <v>1.5263071966125326</v>
+      </c>
+      <c r="AU2">
+        <v>1.5262469615990861</v>
+      </c>
+      <c r="AV2">
+        <v>1.5263009545716171</v>
+      </c>
+      <c r="AW2">
+        <v>1.5263441887643479</v>
+      </c>
+      <c r="AX2">
+        <v>1.5261672201149856</v>
+      </c>
+      <c r="AY2">
+        <v>1.5258450132215851</v>
+      </c>
+      <c r="AZ2">
+        <v>1.5255512281580013</v>
+      </c>
+      <c r="BA2">
+        <v>1.5252667502560493</v>
+      </c>
+      <c r="BB2">
+        <v>1.5248489251275763</v>
+      </c>
+      <c r="BC2">
+        <v>1.5242679496181109</v>
+      </c>
+      <c r="BD2">
+        <v>1.5237471962881441</v>
+      </c>
+      <c r="BE2">
+        <v>1.5233733099193394</v>
+      </c>
+      <c r="BF2">
+        <v>1.5229033942122907</v>
+      </c>
+      <c r="BG2">
+        <v>1.5222785850417042</v>
+      </c>
+      <c r="BH2">
+        <v>1.5216792138532518</v>
+      </c>
+      <c r="BI2">
+        <v>1.5212542403460343</v>
+      </c>
+      <c r="BJ2">
+        <v>1.5209549915627114</v>
+      </c>
+      <c r="BK2">
+        <v>1.5205199592891647</v>
+      </c>
+      <c r="BL2">
+        <v>1.5200168397370246</v>
+      </c>
+      <c r="BM2">
+        <v>1.519707154430022</v>
+      </c>
+      <c r="BN2">
+        <v>1.5194574975022834</v>
+      </c>
+      <c r="BO2">
+        <v>1.5190874952136926</v>
+      </c>
+      <c r="BP2">
+        <v>1.5185507372782112</v>
+      </c>
+      <c r="BQ2">
+        <v>1.5180363211971104</v>
+      </c>
+      <c r="BR2">
+        <v>1.5178226360950546</v>
+      </c>
+      <c r="BS2">
+        <v>1.5175177493677661</v>
+      </c>
+      <c r="BT2">
+        <v>1.5168407007256781</v>
+      </c>
+      <c r="BU2">
+        <v>1.516264922054992</v>
+      </c>
+      <c r="BV2">
+        <v>1.5159592161431157</v>
+      </c>
+      <c r="BW2">
+        <v>1.5157731783138455</v>
+      </c>
+      <c r="BX2">
+        <v>1.5154869807734723</v>
+      </c>
+      <c r="BY2">
+        <v>1.514851147471598</v>
+      </c>
+      <c r="BZ2">
+        <v>1.5145529519975212</v>
+      </c>
+      <c r="CA2">
+        <v>1.5149961207972011</v>
+      </c>
+      <c r="CB2">
+        <v>1.514899886346164</v>
+      </c>
+      <c r="CC2">
+        <v>1.5138483742718316</v>
+      </c>
+      <c r="CD2">
+        <v>1.513330972420017</v>
+      </c>
+      <c r="CE2">
+        <v>1.5141168415135202</v>
+      </c>
+      <c r="CF2">
+        <v>1.5149276650750432</v>
+      </c>
+      <c r="CG2">
+        <v>1.5136461548980926</v>
+      </c>
+      <c r="CH2">
+        <v>1.5101237328779418</v>
+      </c>
+      <c r="CI2">
+        <v>1.5077650022151419</v>
+      </c>
+      <c r="CJ2">
+        <v>1.5107773869134853</v>
+      </c>
+      <c r="CK2">
+        <v>1.5183404969291765</v>
+      </c>
+      <c r="CL2">
+        <v>1.5207019456865558</v>
+      </c>
+      <c r="CM2">
+        <v>1.5031797692426034</v>
+      </c>
+      <c r="CN2">
+        <v>1.4557364782864732</v>
+      </c>
+      <c r="CO2">
+        <v>1.3763480720795631</v>
+      </c>
+      <c r="CP2">
+        <v>1.2670445247921924</v>
+      </c>
+      <c r="CQ2">
+        <v>1.1321672192063503</v>
+      </c>
+      <c r="CR2">
+        <v>0.97877575372190795</v>
+      </c>
+      <c r="CS2">
+        <v>0.81508483367078532</v>
+      </c>
+      <c r="CT2">
+        <v>0.6487664089452142</v>
+      </c>
+      <c r="CU2">
+        <v>0.48668327611806517</v>
+      </c>
+      <c r="CV2">
+        <v>0.33602907362330697</v>
+      </c>
+      <c r="CW2">
+        <v>0.2062990964860692</v>
+      </c>
+      <c r="CX2">
+        <v>0.1083948759173174</v>
+      </c>
+      <c r="CY2">
+        <v>4.7858324503776598E-2</v>
+      </c>
+      <c r="CZ2">
+        <v>1.8821412515957783E-2</v>
+      </c>
+      <c r="DA2">
+        <v>8.2962639729193578E-3</v>
+      </c>
+      <c r="DB2">
+        <v>6.8705951520887593E-3</v>
+      </c>
+      <c r="DC2">
+        <v>8.8793403018316546E-3</v>
+      </c>
+      <c r="DD2">
+        <v>1.0059587743578189E-2</v>
+      </c>
+      <c r="DE2">
+        <v>9.5889398454073373E-3</v>
+      </c>
+      <c r="DF2">
+        <v>8.4880041080658639E-3</v>
+      </c>
+      <c r="DG2">
+        <v>8.0113458891341218E-3</v>
+      </c>
+      <c r="DH2">
+        <v>8.3184224271842366E-3</v>
+      </c>
+      <c r="DI2">
+        <v>8.4818298306327412E-3</v>
+      </c>
+      <c r="DJ2">
+        <v>8.0443360770167723E-3</v>
+      </c>
+      <c r="DK2">
+        <v>7.5316688990723834E-3</v>
+      </c>
+      <c r="DL2">
+        <v>7.6674303139162387E-3</v>
+      </c>
+      <c r="DM2">
+        <v>8.1287947944547884E-3</v>
+      </c>
+      <c r="DN2">
+        <v>8.1127091917667562E-3</v>
+      </c>
+      <c r="DO2">
+        <v>7.6323227262003008E-3</v>
+      </c>
+      <c r="DP2">
+        <v>7.4448976376214164E-3</v>
+      </c>
+      <c r="DQ2">
+        <v>7.7713864060567463E-3</v>
+      </c>
+      <c r="DR2">
+        <v>7.6875965574549855E-3</v>
+      </c>
+      <c r="DS2">
+        <v>7.5428638439906459E-3</v>
+      </c>
+      <c r="DT2">
+        <v>8.7825675002132422E-3</v>
+      </c>
+      <c r="DU2">
+        <v>8.265019327992406E-3</v>
+      </c>
+      <c r="DV2">
+        <v>1.2654127611547791E-2</v>
+      </c>
+      <c r="DW2">
+        <v>1.6125067127777105E-2</v>
+      </c>
+      <c r="DX2">
+        <v>5.5041904752392974E-35</v>
       </c>
     </row>
   </sheetData>
@@ -2089,19 +3824,527 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{4E261BB3-0E66-4719-BE9C-002FE9256592}">
-          <x14:colorSeries rgb="FF000000"/>
-          <x14:colorNegative rgb="FF0070C0"/>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D7EB8D97-A2B5-4769-924B-0EEB8B33B7EA}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF0070C0"/>
-          <x14:colorFirst rgb="FF0070C0"/>
-          <x14:colorLast rgb="FF0070C0"/>
-          <x14:colorHigh rgb="FF0070C0"/>
-          <x14:colorLow rgb="FF0070C0"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!1:1</xm:f>
+              <xm:f>Sheet1!A2:A2</xm:f>
               <xm:sqref>A2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!B2:B2</xm:f>
+              <xm:sqref>B2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!C2:C2</xm:f>
+              <xm:sqref>C2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!D2:D2</xm:f>
+              <xm:sqref>D2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E2:E2</xm:f>
+              <xm:sqref>E2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!F2:F2</xm:f>
+              <xm:sqref>F2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!G2:G2</xm:f>
+              <xm:sqref>G2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!H2:H2</xm:f>
+              <xm:sqref>H2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!I2:I2</xm:f>
+              <xm:sqref>I2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!J2:J2</xm:f>
+              <xm:sqref>J2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!K2:K2</xm:f>
+              <xm:sqref>K2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L2:L2</xm:f>
+              <xm:sqref>L2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M2:M2</xm:f>
+              <xm:sqref>M2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!N2:N2</xm:f>
+              <xm:sqref>N2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!O2:O2</xm:f>
+              <xm:sqref>O2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!P2:P2</xm:f>
+              <xm:sqref>P2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!Q2:Q2</xm:f>
+              <xm:sqref>Q2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!R2:R2</xm:f>
+              <xm:sqref>R2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!S2:S2</xm:f>
+              <xm:sqref>S2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!T2:T2</xm:f>
+              <xm:sqref>T2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!U2:U2</xm:f>
+              <xm:sqref>U2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V2:V2</xm:f>
+              <xm:sqref>V2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!W2:W2</xm:f>
+              <xm:sqref>W2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X2:X2</xm:f>
+              <xm:sqref>X2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!Y2:Y2</xm:f>
+              <xm:sqref>Y2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!Z2:Z2</xm:f>
+              <xm:sqref>Z2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AA2:AA2</xm:f>
+              <xm:sqref>AA2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AB2:AB2</xm:f>
+              <xm:sqref>AB2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AC2:AC2</xm:f>
+              <xm:sqref>AC2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AD2:AD2</xm:f>
+              <xm:sqref>AD2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AE2:AE2</xm:f>
+              <xm:sqref>AE2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AF2:AF2</xm:f>
+              <xm:sqref>AF2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AG2:AG2</xm:f>
+              <xm:sqref>AG2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AH2:AH2</xm:f>
+              <xm:sqref>AH2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AI2:AI2</xm:f>
+              <xm:sqref>AI2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AJ2:AJ2</xm:f>
+              <xm:sqref>AJ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AK2:AK2</xm:f>
+              <xm:sqref>AK2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AL2:AL2</xm:f>
+              <xm:sqref>AL2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AM2:AM2</xm:f>
+              <xm:sqref>AM2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AN2:AN2</xm:f>
+              <xm:sqref>AN2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AO2:AO2</xm:f>
+              <xm:sqref>AO2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AP2:AP2</xm:f>
+              <xm:sqref>AP2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AQ2:AQ2</xm:f>
+              <xm:sqref>AQ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AR2:AR2</xm:f>
+              <xm:sqref>AR2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AS2:AS2</xm:f>
+              <xm:sqref>AS2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AT2:AT2</xm:f>
+              <xm:sqref>AT2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AU2:AU2</xm:f>
+              <xm:sqref>AU2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AV2:AV2</xm:f>
+              <xm:sqref>AV2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AW2:AW2</xm:f>
+              <xm:sqref>AW2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AX2:AX2</xm:f>
+              <xm:sqref>AX2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AY2:AY2</xm:f>
+              <xm:sqref>AY2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!AZ2:AZ2</xm:f>
+              <xm:sqref>AZ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BA2:BA2</xm:f>
+              <xm:sqref>BA2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BB2:BB2</xm:f>
+              <xm:sqref>BB2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BC2:BC2</xm:f>
+              <xm:sqref>BC2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BD2:BD2</xm:f>
+              <xm:sqref>BD2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BE2:BE2</xm:f>
+              <xm:sqref>BE2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BF2:BF2</xm:f>
+              <xm:sqref>BF2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BG2:BG2</xm:f>
+              <xm:sqref>BG2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BH2:BH2</xm:f>
+              <xm:sqref>BH2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BI2:BI2</xm:f>
+              <xm:sqref>BI2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BJ2:BJ2</xm:f>
+              <xm:sqref>BJ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BK2:BK2</xm:f>
+              <xm:sqref>BK2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BL2:BL2</xm:f>
+              <xm:sqref>BL2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BM2:BM2</xm:f>
+              <xm:sqref>BM2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BN2:BN2</xm:f>
+              <xm:sqref>BN2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BO2:BO2</xm:f>
+              <xm:sqref>BO2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BP2:BP2</xm:f>
+              <xm:sqref>BP2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BQ2:BQ2</xm:f>
+              <xm:sqref>BQ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BR2:BR2</xm:f>
+              <xm:sqref>BR2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BS2:BS2</xm:f>
+              <xm:sqref>BS2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BT2:BT2</xm:f>
+              <xm:sqref>BT2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BU2:BU2</xm:f>
+              <xm:sqref>BU2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BV2:BV2</xm:f>
+              <xm:sqref>BV2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BW2:BW2</xm:f>
+              <xm:sqref>BW2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BX2:BX2</xm:f>
+              <xm:sqref>BX2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BY2:BY2</xm:f>
+              <xm:sqref>BY2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!BZ2:BZ2</xm:f>
+              <xm:sqref>BZ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CA2:CA2</xm:f>
+              <xm:sqref>CA2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CB2:CB2</xm:f>
+              <xm:sqref>CB2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CC2:CC2</xm:f>
+              <xm:sqref>CC2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CD2:CD2</xm:f>
+              <xm:sqref>CD2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CE2:CE2</xm:f>
+              <xm:sqref>CE2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CF2:CF2</xm:f>
+              <xm:sqref>CF2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CG2:CG2</xm:f>
+              <xm:sqref>CG2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CH2:CH2</xm:f>
+              <xm:sqref>CH2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CI2:CI2</xm:f>
+              <xm:sqref>CI2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CJ2:CJ2</xm:f>
+              <xm:sqref>CJ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CK2:CK2</xm:f>
+              <xm:sqref>CK2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CL2:CL2</xm:f>
+              <xm:sqref>CL2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CM2:CM2</xm:f>
+              <xm:sqref>CM2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CN2:CN2</xm:f>
+              <xm:sqref>CN2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CO2:CO2</xm:f>
+              <xm:sqref>CO2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CP2:CP2</xm:f>
+              <xm:sqref>CP2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CQ2:CQ2</xm:f>
+              <xm:sqref>CQ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CR2:CR2</xm:f>
+              <xm:sqref>CR2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CS2:CS2</xm:f>
+              <xm:sqref>CS2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CT2:CT2</xm:f>
+              <xm:sqref>CT2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CU2:CU2</xm:f>
+              <xm:sqref>CU2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CV2:CV2</xm:f>
+              <xm:sqref>CV2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CW2:CW2</xm:f>
+              <xm:sqref>CW2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CX2:CX2</xm:f>
+              <xm:sqref>CX2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CY2:CY2</xm:f>
+              <xm:sqref>CY2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!CZ2:CZ2</xm:f>
+              <xm:sqref>CZ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DA2:DA2</xm:f>
+              <xm:sqref>DA2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DB2:DB2</xm:f>
+              <xm:sqref>DB2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DC2:DC2</xm:f>
+              <xm:sqref>DC2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DD2:DD2</xm:f>
+              <xm:sqref>DD2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DE2:DE2</xm:f>
+              <xm:sqref>DE2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DF2:DF2</xm:f>
+              <xm:sqref>DF2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DG2:DG2</xm:f>
+              <xm:sqref>DG2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DH2:DH2</xm:f>
+              <xm:sqref>DH2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DI2:DI2</xm:f>
+              <xm:sqref>DI2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DJ2:DJ2</xm:f>
+              <xm:sqref>DJ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DK2:DK2</xm:f>
+              <xm:sqref>DK2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DL2:DL2</xm:f>
+              <xm:sqref>DL2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DM2:DM2</xm:f>
+              <xm:sqref>DM2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DN2:DN2</xm:f>
+              <xm:sqref>DN2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DO2:DO2</xm:f>
+              <xm:sqref>DO2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DP2:DP2</xm:f>
+              <xm:sqref>DP2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DQ2:DQ2</xm:f>
+              <xm:sqref>DQ2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DR2:DR2</xm:f>
+              <xm:sqref>DR2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DS2:DS2</xm:f>
+              <xm:sqref>DS2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DT2:DT2</xm:f>
+              <xm:sqref>DT2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DU2:DU2</xm:f>
+              <xm:sqref>DU2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DV2:DV2</xm:f>
+              <xm:sqref>DV2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DW2:DW2</xm:f>
+              <xm:sqref>DW2</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!DX2:DX2</xm:f>
+              <xm:sqref>DX2</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>